<commit_message>
COM_FR, CEFF-O, InputActivityRatio and OutputActivityRatio
</commit_message>
<xml_diff>
--- a/SuppXls/Scen_Ose_param.xlsx
+++ b/SuppXls/Scen_Ose_param.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Veda2.0_localhost_2.17.1.1\Veda\Veda_models\Demo_models\DemoS_003\SuppXls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78AEEB0-1486-437F-A843-652FA7BD9DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8598EAE0-CB05-4D23-B9AF-32752045BA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INS" sheetId="2" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="48">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -233,6 +233,33 @@
   </si>
   <si>
     <t>other_indexes</t>
+  </si>
+  <si>
+    <t>OutputActivityRatio</t>
+  </si>
+  <si>
+    <t>IRE</t>
+  </si>
+  <si>
+    <t>NRG</t>
+  </si>
+  <si>
+    <t>top_check</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>InputActivityRatio</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>CEFF</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -362,7 +389,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -384,6 +411,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,20 +752,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -747,12 +774,12 @@
     <col min="15" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>16</v>
       </c>
@@ -765,7 +792,7 @@
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
@@ -782,7 +809,7 @@
         <v>38</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>18</v>
@@ -811,8 +838,11 @@
       <c r="P3" s="14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>36</v>
       </c>
@@ -826,7 +856,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>36</v>
       </c>
@@ -838,6 +868,69 @@
       </c>
       <c r="I5" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>